<commit_message>
feat: :sparkles: Uptaded a link
</commit_message>
<xml_diff>
--- a/public/Tableau des compétences.xlsx
+++ b/public/Tableau des compétences.xlsx
@@ -23,24 +23,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
   <si>
-    <t xml:space="preserve">SESSION 2023</t>
+    <t xml:space="preserve">SESSION 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
-    <t xml:space="preserve">NOM et prénom : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centre de formation :</t>
+    <t xml:space="preserve">NOM et prénom : BEIRADE Ilyes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="18"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">N° candidat : </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">01947268117</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre de formation : Lycée Jacques Brel</t>
   </si>
   <si>
     <t xml:space="preserve">Option :</t>
@@ -52,7 +72,7 @@
     <t xml:space="preserve">☑ SLAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Adresse URL du portfolio :</t>
+    <t xml:space="preserve">Adresse URL du portfolio : https://portfolio-ilyes.vercel.app/</t>
   </si>
   <si>
     <t xml:space="preserve">Compétences mises en œuvre
@@ -119,54 +139,95 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Création d’Autoclean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/09/2023 au 03/10/2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Continuation d’SGRC</t>
+    <t xml:space="preserve">GLPI (Gestionnaire de parc informatique)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/09/2022 au 12/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renaissance urbaine (Projet Association)</t>
   </si>
   <si>
     <t xml:space="preserve">03/09/2023 au 12/01/2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Création de « Manif »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installation d’un GLPI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/09/2022 au 12/01/2023</t>
+    <t xml:space="preserve">SGRC (Application web)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCS (Application web)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/03/2024 au 05/03/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track-It (Projet mobile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/02/2024 à Aujourd’hui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autoclean (Site web)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/10/2023 à Aujourd’hui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfollio (Site web)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/09/2023 au 02/04/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compte LinkedIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/09/2021 à Aujourd’hui</t>
   </si>
   <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
-    <t xml:space="preserve">Refactoring d’INOLIB</t>
+    <t xml:space="preserve">INOLIB (Site web)</t>
   </si>
   <si>
     <t xml:space="preserve">15/05/2023 au 23/06/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">Création d’InoFormation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création d’InoTest</t>
+    <t xml:space="preserve">InoTest (Librairie)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InoFormation (Site web)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exposant au salon Les Halles du Numérique</t>
   </si>
   <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessible Components (Librairie)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/01/2024 au 23/02/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessible Quiz (Site web)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant au salon Tech&amp;Fest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -198,6 +259,30 @@
     <font>
       <b val="true"/>
       <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -232,7 +317,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -242,18 +327,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -546,7 +619,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -570,11 +643,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -607,115 +677,90 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Euro" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -729,7 +774,7 @@
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF00000A"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
@@ -787,14 +832,14 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="70.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="9" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="44" style="1" width="10.85"/>
@@ -940,292 +985,388 @@
       <c r="B9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+      <c r="C9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+        <v>29</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
+        <v>32</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
+      <c r="A13" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
+      <c r="A14" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="A15" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
+      <c r="A16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18"/>
       <c r="B17" s="19"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18"/>
       <c r="B18" s="19"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" s="16" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="A19" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
     </row>
     <row r="20" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="21"/>
     </row>
     <row r="21" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
+        <v>45</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
+      <c r="A23" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="19"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" s="16" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
+      <c r="A27" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
     </row>
     <row r="28" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
+      <c r="A28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="21"/>
     </row>
     <row r="29" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
+      <c r="A29" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
+      <c r="A30" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="19"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
     </row>
     <row r="32" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" s="16" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="32"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="26"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A1:F1"/>
@@ -1241,6 +1382,9 @@
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" display="Adresse URL du portfolio : https://portfolio-ilyes.vercel.app/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>